<commit_message>
Adding extra column in base table DBA_All_servers
</commit_message>
<xml_diff>
--- a/DBA_Automon_Details.xlsx
+++ b/DBA_Automon_Details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2019-2020-before-UK-in-UK\TCS_Ageas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AutoMon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>SP Name</t>
   </si>
@@ -161,36 +161,21 @@
     <t>New login and DB creation</t>
   </si>
   <si>
-    <t>Maintenance mode review</t>
-  </si>
-  <si>
-    <t>Error report of Automon tool</t>
-  </si>
-  <si>
     <t>AlwaysOn health check</t>
   </si>
   <si>
     <t>AlwaysOn quorum health check</t>
   </si>
   <si>
-    <t>Recovery model check</t>
-  </si>
-  <si>
     <t>Memory high alert</t>
   </si>
   <si>
     <t>CPU high alert</t>
   </si>
   <si>
-    <t>Disk free space alert backup drive</t>
-  </si>
-  <si>
     <t>SQL Service ping health status</t>
   </si>
   <si>
-    <t>Auto maintenance mode after 5 alert</t>
-  </si>
-  <si>
     <t>EXEC [DBAData].dbo.usp_linked_server_status_Check</t>
   </si>
   <si>
@@ -200,9 +185,6 @@
     <t>Usp_agent_status</t>
   </si>
   <si>
-    <t>Maintenance window release</t>
-  </si>
-  <si>
     <t>Ad-hoc</t>
   </si>
   <si>
@@ -215,16 +197,43 @@
     <t>Daily 6 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">Backup share path alert </t>
-  </si>
-  <si>
     <t>EXEC [DBAdata].dbo.[Usp_Alwayson_Lag_Monitoring]</t>
   </si>
   <si>
-    <t>AutoMon Job Disbaled alert</t>
-  </si>
-  <si>
     <t xml:space="preserve">update DBADATA.DBO.DBA_ALL_SERVERS set svr_status ='Running' where svr_status ='not ping_U' </t>
+  </si>
+  <si>
+    <t>Recovery model check for non production</t>
+  </si>
+  <si>
+    <t>Recovery model check for production</t>
+  </si>
+  <si>
+    <t>Auto maintenance mode after 5 ping health fails</t>
+  </si>
+  <si>
+    <t>Maintenance window release daily morning</t>
+  </si>
+  <si>
+    <t>Disk free space percentage alert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backup share path free space alert </t>
+  </si>
+  <si>
+    <t>AlwaysOn out of sync lag check</t>
+  </si>
+  <si>
+    <t>AutoMon SQL server not running status</t>
+  </si>
+  <si>
+    <t>Error report of AutoMon tool</t>
+  </si>
+  <si>
+    <t>Write script to get AutoMon Job Disabled alert</t>
+  </si>
+  <si>
+    <t>Configure the job based on your requirements</t>
   </si>
 </sst>
 </file>
@@ -262,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -285,11 +294,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -300,6 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +602,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,7 +640,7 @@
       <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -633,7 +654,7 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -690,7 +711,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -704,7 +725,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -717,7 +738,7 @@
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -732,7 +753,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -760,21 +781,21 @@
         <v>20</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -785,7 +806,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>42</v>
@@ -799,7 +820,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>43</v>
@@ -807,16 +828,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,24 +848,24 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -855,38 +876,38 @@
         <v>15</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -897,10 +918,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -913,8 +934,8 @@
       <c r="C23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>46</v>
+      <c r="D23" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -928,12 +949,12 @@
         <v>26</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>25</v>
@@ -942,7 +963,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -955,8 +976,8 @@
       <c r="C26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>49</v>
+      <c r="D26" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -970,7 +991,7 @@
         <v>33</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -984,7 +1005,12 @@
         <v>33</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>